<commit_message>
fixed README.md expriment purpose
</commit_message>
<xml_diff>
--- a/demo/シミュレーション結果.xlsx
+++ b/demo/シミュレーション結果.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="28035" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="結果一覧" sheetId="1" r:id="rId1"/>
-    <sheet name="t検定結果" sheetId="2" r:id="rId2"/>
-    <sheet name="全体用演算" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="本実験の目的" sheetId="4" r:id="rId1"/>
+    <sheet name="結果一覧" sheetId="1" r:id="rId2"/>
+    <sheet name="t検定結果" sheetId="2" r:id="rId3"/>
+    <sheet name="全体用演算" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>ステップ数</t>
     <rPh sb="4" eb="5">
@@ -459,6 +460,62 @@
   </si>
   <si>
     <t>改善前</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■本プロジェクトの実験の目的</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ただ、QUBOを解く式が大きいため、GoogleColab上では実現可能な時間で計算は不可能だった。</t>
+  </si>
+  <si>
+    <t>改善前のQUBOの式</t>
+    <rPh sb="0" eb="3">
+      <t>カイゼンマエ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2つやりたい実験があります。</t>
+    <rPh sb="6" eb="8">
+      <t>ジッケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一つ目は、実現可能な時間で計算できるものか見てみたい。（特に改善前において）</t>
+  </si>
+  <si>
+    <t>二つ目は、改善前の目的項はQAで解くような式になっていなかった。改善後として、QAの特徴を更に活かせるような式を追加した。そこに効果があるか見てみたい。</t>
+  </si>
+  <si>
+    <t>その際にt検定を用いて、効果があるか検証した。</t>
+    <rPh sb="2" eb="3">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ケンテイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>モチ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>コウカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ケンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>今回、そのステップ数（解く回数）に効果があるか検証したい。</t>
+    <rPh sb="23" eb="25">
+      <t>ケンショウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -466,7 +523,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,6 +561,68 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF1F2328"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF1F2328"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="5">
@@ -644,7 +763,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,6 +809,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -698,6 +823,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,6 +854,201 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>312657</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>84783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="1219200"/>
+          <a:ext cx="13342857" cy="7533333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="円形吹き出し 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8429624" y="3171824"/>
+          <a:ext cx="3914775" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeEllipseCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -65519"/>
+            <a:gd name="adj2" fmla="val -18618"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>目的項にロボット</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>h1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>と</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>h2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>が絡んでないため</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>QA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の特徴を活かしているとは言えない</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="円形吹き出し 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10506075" y="6677025"/>
+          <a:ext cx="3914775" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeEllipseCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -65519"/>
+            <a:gd name="adj2" fmla="val -18618"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>制約項①②については、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>QA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の特徴を活かした式である。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1000,9 +1338,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24">
+      <c r="A1" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24">
+      <c r="A2" s="16"/>
+      <c r="B2" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24">
+      <c r="B3" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24">
+      <c r="B4" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.25">
+      <c r="B5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="17.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25">
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" ht="17.25">
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" ht="17.25">
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" ht="17.25">
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" ht="17.25">
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" ht="17.25">
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" ht="17.25">
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" ht="17.25">
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="17.25">
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" ht="17.25">
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="2:2" ht="17.25">
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="2:2" ht="17.25">
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="2:2" ht="17.25">
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="2:2" ht="17.25">
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="2:2" ht="17.25">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="2:2" ht="17.25">
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="2:2" ht="17.25">
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="2:2" ht="17.25">
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="2:2" ht="17.25">
+      <c r="B25" s="15"/>
+    </row>
+    <row r="26" spans="2:2" ht="17.25">
+      <c r="B26" s="15"/>
+    </row>
+    <row r="27" spans="2:2" ht="17.25">
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="2:2" ht="17.25">
+      <c r="B28" s="15"/>
+    </row>
+    <row r="29" spans="2:2" ht="17.25">
+      <c r="B29" s="15"/>
+    </row>
+    <row r="30" spans="2:2" ht="17.25">
+      <c r="B30" s="15"/>
+    </row>
+    <row r="31" spans="2:2" ht="17.25">
+      <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="2:2" ht="17.25">
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="2:2" ht="17.25">
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="2:2" ht="17.25">
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="2:2" ht="17.25">
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="2:2" ht="17.25">
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="2:2" ht="17.25">
+      <c r="B37" s="15"/>
+    </row>
+    <row r="38" spans="2:2" ht="17.25">
+      <c r="B38" s="15"/>
+    </row>
+    <row r="39" spans="2:2" ht="17.25">
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="2:2" ht="17.25">
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="2:2" ht="17.25">
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="2:2" ht="17.25">
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="2:2" ht="17.25">
+      <c r="B43" s="15"/>
+    </row>
+    <row r="44" spans="2:2" ht="17.25">
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="2:2" ht="17.25">
+      <c r="B45" s="15"/>
+    </row>
+    <row r="46" spans="2:2" ht="17.25">
+      <c r="B46" s="15"/>
+    </row>
+    <row r="47" spans="2:2" ht="17.25">
+      <c r="B47" s="15"/>
+    </row>
+    <row r="48" spans="2:2" ht="17.25">
+      <c r="B48" s="15"/>
+    </row>
+    <row r="49" spans="2:3" ht="20.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="17.25">
+      <c r="C50" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="17.25">
+      <c r="C51" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1017,37 +1548,37 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
@@ -1693,7 +2224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M47"/>
   <sheetViews>
@@ -2119,7 +2650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -2135,10 +2666,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">

</xml_diff>